<commit_message>
Random 10 quiz q's works
</commit_message>
<xml_diff>
--- a/quiz/backend/questions.xlsx
+++ b/quiz/backend/questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\owencooke15\TestReact\test\backend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\owencooke15\TestReact\quiz\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{081A91BB-A2A6-4E84-B923-8ED0CA7112FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC9D40F-39A5-4D9F-ADFA-E2A7436042FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="questions" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="98">
   <si>
     <t>Question</t>
   </si>
@@ -35,13 +35,292 @@
   </si>
   <si>
     <t>Incorrect Option 3</t>
+  </si>
+  <si>
+    <t>Less than 4</t>
+  </si>
+  <si>
+    <t>150 000</t>
+  </si>
+  <si>
+    <t>262 130</t>
+  </si>
+  <si>
+    <t>9 and a half</t>
+  </si>
+  <si>
+    <t>Otter</t>
+  </si>
+  <si>
+    <t>Falcon</t>
+  </si>
+  <si>
+    <t>Grizzly Bear</t>
+  </si>
+  <si>
+    <t>Orca</t>
+  </si>
+  <si>
+    <t>Drake Lake</t>
+  </si>
+  <si>
+    <t>Osoyoos Lake</t>
+  </si>
+  <si>
+    <t>Lake Lebron</t>
+  </si>
+  <si>
+    <t>Lake Waffles</t>
+  </si>
+  <si>
+    <t>Canuck Island</t>
+  </si>
+  <si>
+    <t>Mount Island</t>
+  </si>
+  <si>
+    <t>Vancouver Island</t>
+  </si>
+  <si>
+    <t>Surrey Island</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>Second</t>
+  </si>
+  <si>
+    <t>Third</t>
+  </si>
+  <si>
+    <t>Fourth</t>
+  </si>
+  <si>
+    <t>One for each person</t>
+  </si>
+  <si>
+    <t>Mount Logan</t>
+  </si>
+  <si>
+    <t>Mount Everest</t>
+  </si>
+  <si>
+    <t>Mount Kilimanjaro</t>
+  </si>
+  <si>
+    <t>Mount Tacos</t>
+  </si>
+  <si>
+    <t>Black Bear</t>
+  </si>
+  <si>
+    <t>Panda Bear</t>
+  </si>
+  <si>
+    <t>Kermode Bear</t>
+  </si>
+  <si>
+    <t>apples and bananas</t>
+  </si>
+  <si>
+    <t>flying bananas and talking kiwis</t>
+  </si>
+  <si>
+    <t>cranberries and blueberries</t>
+  </si>
+  <si>
+    <t>strawberries and oranges</t>
+  </si>
+  <si>
+    <t>Loch Ness Monster river</t>
+  </si>
+  <si>
+    <t>Mississippi River</t>
+  </si>
+  <si>
+    <t>Fraser River</t>
+  </si>
+  <si>
+    <t>Columbia River</t>
+  </si>
+  <si>
+    <t>25 725 miles</t>
+  </si>
+  <si>
+    <t>25 725 kilometers</t>
+  </si>
+  <si>
+    <t>600 kilometers</t>
+  </si>
+  <si>
+    <t>50 meters</t>
+  </si>
+  <si>
+    <t>9.5% </t>
+  </si>
+  <si>
+    <t>Atlantic Ocean</t>
+  </si>
+  <si>
+    <t>Indian Ocean</t>
+  </si>
+  <si>
+    <t>Arctic Ocean</t>
+  </si>
+  <si>
+    <t>Pacific Ocean</t>
+  </si>
+  <si>
+    <t>Montana</t>
+  </si>
+  <si>
+    <t>Minnesota</t>
+  </si>
+  <si>
+    <t>North Carolina</t>
+  </si>
+  <si>
+    <t>Alaska</t>
+  </si>
+  <si>
+    <t>1200 kilometers</t>
+  </si>
+  <si>
+    <t>500 footlong Subway sandwiches</t>
+  </si>
+  <si>
+    <t>2000 miles</t>
+  </si>
+  <si>
+    <t>1 light year </t>
+  </si>
+  <si>
+    <t>20 000</t>
+  </si>
+  <si>
+    <t>400 000</t>
+  </si>
+  <si>
+    <t>40 000</t>
+  </si>
+  <si>
+    <t>humpback whale</t>
+  </si>
+  <si>
+    <t>orca whale</t>
+  </si>
+  <si>
+    <t>whale shark</t>
+  </si>
+  <si>
+    <t>blue whale</t>
+  </si>
+  <si>
+    <t>geese</t>
+  </si>
+  <si>
+    <t>common loon</t>
+  </si>
+  <si>
+    <t>beaver </t>
+  </si>
+  <si>
+    <t>moose</t>
+  </si>
+  <si>
+    <t>maple tree</t>
+  </si>
+  <si>
+    <t>birch tree</t>
+  </si>
+  <si>
+    <t>lodgepole pine</t>
+  </si>
+  <si>
+    <t>oak tree</t>
+  </si>
+  <si>
+    <t>British Columbia is a top three province in producing which fruits?</t>
+  </si>
+  <si>
+    <t>British Columbia is covered in ______ kilometers squared of forest.</t>
+  </si>
+  <si>
+    <t>British Columbia is home to the only ______ sanctuary in Canada.</t>
+  </si>
+  <si>
+    <t>There are ______ cougars in British Columbia.</t>
+  </si>
+  <si>
+    <t>The warmest freshwater lake in Canada is?</t>
+  </si>
+  <si>
+    <t>The largest island in British Columbia is?</t>
+  </si>
+  <si>
+    <t>British Columbia is the ______ largest province in Canada.</t>
+  </si>
+  <si>
+    <t>British Columbia has ______ rivers.</t>
+  </si>
+  <si>
+    <t>The tallest mountain in British Columbia is?</t>
+  </si>
+  <si>
+    <t>The national animal of British Columbia is?</t>
+  </si>
+  <si>
+    <t>The longest river in British Columbia is?</t>
+  </si>
+  <si>
+    <t>BC has a coastal line that stretches how far?</t>
+  </si>
+  <si>
+    <t>BC has ______ provincial parks.</t>
+  </si>
+  <si>
+    <t>There are more than ______ Indigenous groups in British Columbia.</t>
+  </si>
+  <si>
+    <t>British Columbia’s population is?</t>
+  </si>
+  <si>
+    <t>British Columbia covers ______ of Canada’s area.</t>
+  </si>
+  <si>
+    <t>British Columbia borders which body of water?</t>
+  </si>
+  <si>
+    <t>The US state that borders British Columbia from the north is?</t>
+  </si>
+  <si>
+    <t>From north to south, British Columbia is how long?</t>
+  </si>
+  <si>
+    <t>There are ______ islands in British Columbia.</t>
+  </si>
+  <si>
+    <t>British Columbia has ______ Indigenous languages.</t>
+  </si>
+  <si>
+    <t>British Columbia is so big, it actually has  ______ different time zones.</t>
+  </si>
+  <si>
+    <t>The most popular whale in British Columbia is?</t>
+  </si>
+  <si>
+    <t>British Columbia has this animal called the ______, which is on the one dollar coin.</t>
+  </si>
+  <si>
+    <t>The ______ is the most common tree in British Columbia.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,6 +454,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="33">
@@ -518,8 +803,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -874,16 +1168,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" customWidth="1"/>
+    <col min="1" max="1" width="84" customWidth="1"/>
     <col min="2" max="2" width="18.88671875" customWidth="1"/>
     <col min="3" max="3" width="19.44140625" customWidth="1"/>
     <col min="4" max="4" width="21.21875" customWidth="1"/>
@@ -907,7 +1201,460 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3500</v>
+      </c>
+      <c r="C4" s="2">
+        <v>5300</v>
+      </c>
+      <c r="D4" s="2">
+        <v>530</v>
+      </c>
+      <c r="E4" s="2">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="2">
+        <v>20</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="2">
+        <v>17</v>
+      </c>
+      <c r="E8" s="2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1031</v>
+      </c>
+      <c r="C14" s="2">
+        <v>783</v>
+      </c>
+      <c r="D14" s="2">
+        <v>204</v>
+      </c>
+      <c r="E14" s="2">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" s="2">
+        <v>200</v>
+      </c>
+      <c r="C15" s="2">
+        <v>250</v>
+      </c>
+      <c r="D15" s="2">
+        <v>300</v>
+      </c>
+      <c r="E15" s="2">
+        <v>234923572695835</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="2">
+        <v>5</v>
+      </c>
+      <c r="C16" s="2">
+        <v>3</v>
+      </c>
+      <c r="D16" s="2">
+        <v>36</v>
+      </c>
+      <c r="E16" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.81</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E21" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B22" s="2">
+        <v>34</v>
+      </c>
+      <c r="C22" s="2">
+        <v>36</v>
+      </c>
+      <c r="D22" s="2">
+        <v>18</v>
+      </c>
+      <c r="E22" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B23" s="2">
+        <v>2</v>
+      </c>
+      <c r="C23" s="2">
+        <v>-1</v>
+      </c>
+      <c r="D23" s="2">
+        <v>5</v>
+      </c>
+      <c r="E23" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="2"/>
+    </row>
+    <row r="30" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="2"/>
+    </row>
+    <row r="33" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="2"/>
+    </row>
+    <row r="34" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="2"/>
+    </row>
+    <row r="35" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>